<commit_message>
Just for recording first implementation of VeeValidate v4.x adaptation.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoVeeValidateResourceBundle.xlsx
+++ b/meta/program/BlancoVeeValidateResourceBundle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoVeeValidate/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16BD537D-D6CA-7348-B90C-F31E162A4804}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DB32C4-27BF-9745-9655-08F7A7A81489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="2260" windowWidth="28800" windowHeight="17540" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23360" yWindow="8800" windowWidth="28800" windowHeight="17540" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ja" sheetId="9" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="152">
   <si>
     <t>説明</t>
     <rPh sb="0" eb="2">
@@ -680,28 +680,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>XML2SOURCE_FILE.VALIDATE.RULE.SCHEMA</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>VeeValidateのValidateRuleSchemaの実装クラスです。</t>
-    <rPh sb="31" eb="33">
-      <t xml:space="preserve">ジッソウ </t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>XML2SOURCE_FILE.VALIDATE.MESSAGE</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>VeeValidateのカスタムメッセージを定義するクラスです。</t>
-    <rPh sb="22" eb="24">
-      <t xml:space="preserve">テイギ </t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>XML2SOURCE_FILE.ERR007</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -722,6 +700,182 @@
       <t>メッセージク</t>
     </rPh>
     <rPh sb="9" eb="11">
+      <t xml:space="preserve">テイギ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XML2SOURCE_FILE.VALIDATE.REDEFINE.TYPES</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>この型はVeeValidate内で定義されていますがexportされていないので再定義しています。</t>
+    <rPh sb="2" eb="3">
+      <t xml:space="preserve">カタ </t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t xml:space="preserve">テイギ </t>
+    </rPh>
+    <rPh sb="40" eb="43">
+      <t xml:space="preserve">サイテイギ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FIELD の項目名（name）またはラベル（label）</t>
+    <rPh sb="7" eb="8">
+      <t xml:space="preserve">コウモクメイ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FIELD の現在の値</t>
+    <rPh sb="6" eb="7">
+      <t>ノ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t xml:space="preserve">ゲンザイノ </t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t xml:space="preserve">アタイ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FORM 内の他の値</t>
+    <rPh sb="5" eb="6">
+      <t xml:space="preserve">ナイノ </t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>タノ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t xml:space="preserve">アタイ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ルール名</t>
+    <rPh sb="3" eb="4">
+      <t xml:space="preserve">メイ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ルールのパラメータ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ルールの名前とパラメータを表すインタフェイスです。</t>
+    <rPh sb="4" eb="6">
+      <t xml:space="preserve">ナマエト </t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t xml:space="preserve">アラワス </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XML2SOURCE_FILE.VALIDATION.META.INFO.FIELD</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XML2SOURCE_FILE.VALIDATION.META.INFO.VALUE</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XML2SOURCE_FILE.VALIDATION.META.INFO.FORM</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XML2SOURCE_FILE.VALIDATION.META.INFO.RULE.NAME</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XML2SOURCE_FILE.VALIDATION.META.INFO.RULE.PARAMS</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XML2SOURCE_FILE.VALIDATION.META.INFO.RULE</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>VeeValidateのカスタムメッセージを定義するクラスです。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XML2SOURCE_FILE.VALIDATION.MESSAGE</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XML2SOURCE_FILE.VALIDATION.INTERPORATOR.PARAM01</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XML2SOURCE_FILE.VALIDATION.INTERPORATOR.PARAM02</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XML2SOURCE_FILE.VALIDATION.INTERPORATOR.LANGDOC</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>vee-validate/i18n で定義されたメッセージテンプレートのプレースホルダを値に置き換えます。</t>
+    <rPh sb="19" eb="21">
+      <t xml:space="preserve">テイギ </t>
+    </rPh>
+    <rPh sb="44" eb="45">
+      <t xml:space="preserve">アタイニ </t>
+    </rPh>
+    <rPh sb="46" eb="47">
+      <t xml:space="preserve">オキカエマス </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メッセージのテンプレートです。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>プレースホルダと置換される値です。</t>
+    <rPh sb="8" eb="10">
+      <t xml:space="preserve">チカｎ </t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t xml:space="preserve">アタイ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XML2SOURCE_FILE.VALIDATION.INTERPORATOR.RETURN</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>プレースホルダ置換後のメッセージを返します。</t>
+    <rPh sb="7" eb="9">
+      <t xml:space="preserve">チカンゴノ </t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t xml:space="preserve">ゴ </t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t xml:space="preserve">カエシマス。 </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XML2SOURCE_FILE.VALIDATION.CONFIG.OPTIONS</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>configure 関数に渡すオプションの定義です。</t>
+    <rPh sb="10" eb="12">
+      <t xml:space="preserve">カンスウニ </t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t xml:space="preserve">ワタス </t>
+    </rPh>
+    <rPh sb="21" eb="23">
       <t xml:space="preserve">テイギ </t>
     </rPh>
     <phoneticPr fontId="1"/>
@@ -1659,19 +1813,20 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I98"/>
+  <dimension ref="A1:I110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="5" style="12" customWidth="1"/>
-    <col min="2" max="2" width="22.1640625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="48.83203125" style="12" customWidth="1"/>
     <col min="3" max="3" width="11.1640625" style="12" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" style="12" customWidth="1"/>
-    <col min="5" max="7" width="22.1640625" style="12" customWidth="1"/>
+    <col min="5" max="6" width="22.1640625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="53.5" style="12" customWidth="1"/>
     <col min="8" max="16384" width="9" style="12"/>
   </cols>
   <sheetData>
@@ -1830,7 +1985,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="28">
-        <f t="shared" ref="A17:A30" si="0">A16+1</f>
+        <f t="shared" ref="A17:A80" si="0">ROW() - 14</f>
         <v>3</v>
       </c>
       <c r="B17" s="23"/>
@@ -2033,7 +2188,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="28">
-        <f t="shared" ref="A31:A94" si="1">ROW() - 14</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B31" s="23" t="s">
@@ -2049,7 +2204,7 @@
     </row>
     <row r="32" spans="1:9" s="41" customFormat="1">
       <c r="A32" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B32" s="36" t="s">
@@ -2067,7 +2222,7 @@
     </row>
     <row r="33" spans="1:9" s="41" customFormat="1">
       <c r="A33" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B33" s="36" t="s">
@@ -2085,7 +2240,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B34" s="23"/>
@@ -2097,7 +2252,7 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B35" s="23" t="s">
@@ -2113,7 +2268,7 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B36" s="23" t="s">
@@ -2129,7 +2284,7 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B37" s="23"/>
@@ -2141,7 +2296,7 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B38" s="23" t="s">
@@ -2157,7 +2312,7 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B39" s="23" t="s">
@@ -2173,7 +2328,7 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B40" s="23" t="s">
@@ -2189,7 +2344,7 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B41" s="23"/>
@@ -2201,7 +2356,7 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B42" s="23" t="s">
@@ -2217,7 +2372,7 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B43" s="23" t="s">
@@ -2233,7 +2388,7 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B44" s="23" t="s">
@@ -2249,7 +2404,7 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B45" s="23" t="s">
@@ -2265,7 +2420,7 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B46" s="23"/>
@@ -2277,7 +2432,7 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="B47" s="23"/>
@@ -2291,7 +2446,7 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="B48" s="23"/>
@@ -2305,7 +2460,7 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="B49" s="23"/>
@@ -2319,7 +2474,7 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="B50" s="23"/>
@@ -2331,7 +2486,7 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="B51" s="23"/>
@@ -2345,7 +2500,7 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="B52" s="23" t="s">
@@ -2361,7 +2516,7 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>39</v>
       </c>
       <c r="B53" s="23" t="s">
@@ -2377,7 +2532,7 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="B54" s="23" t="s">
@@ -2393,7 +2548,7 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="B55" s="23" t="s">
@@ -2409,7 +2564,7 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="B56" s="23" t="s">
@@ -2425,7 +2580,7 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="B57" s="23" t="s">
@@ -2441,14 +2596,14 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44</v>
       </c>
       <c r="B58" s="23" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C58" s="20" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D58" s="21"/>
       <c r="E58" s="21"/>
@@ -2457,14 +2612,14 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="B59" s="23" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C59" s="20" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D59" s="21"/>
       <c r="E59" s="21"/>
@@ -2473,7 +2628,7 @@
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
       <c r="B60" s="23"/>
@@ -2485,7 +2640,7 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>47</v>
       </c>
       <c r="B61" s="23" t="s">
@@ -2501,7 +2656,7 @@
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="B62" s="23" t="s">
@@ -2517,7 +2672,7 @@
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="B63" s="23" t="s">
@@ -2533,7 +2688,7 @@
     </row>
     <row r="64" spans="1:7">
       <c r="A64" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="B64" s="23"/>
@@ -2545,7 +2700,7 @@
     </row>
     <row r="65" spans="1:7">
       <c r="A65" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>51</v>
       </c>
       <c r="B65" s="23" t="s">
@@ -2561,7 +2716,7 @@
     </row>
     <row r="66" spans="1:7">
       <c r="A66" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
       <c r="B66" s="23" t="s">
@@ -2577,7 +2732,7 @@
     </row>
     <row r="67" spans="1:7">
       <c r="A67" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>53</v>
       </c>
       <c r="B67" s="23" t="s">
@@ -2593,7 +2748,7 @@
     </row>
     <row r="68" spans="1:7">
       <c r="A68" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="B68" s="23"/>
@@ -2605,7 +2760,7 @@
     </row>
     <row r="69" spans="1:7">
       <c r="A69" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="B69" s="23" t="s">
@@ -2621,7 +2776,7 @@
     </row>
     <row r="70" spans="1:7">
       <c r="A70" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="B70" s="23" t="s">
@@ -2637,7 +2792,7 @@
     </row>
     <row r="71" spans="1:7">
       <c r="A71" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="B71" s="23" t="s">
@@ -2653,7 +2808,7 @@
     </row>
     <row r="72" spans="1:7">
       <c r="A72" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="B72" s="23" t="s">
@@ -2669,7 +2824,7 @@
     </row>
     <row r="73" spans="1:7">
       <c r="A73" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>59</v>
       </c>
       <c r="B73" s="23"/>
@@ -2681,7 +2836,7 @@
     </row>
     <row r="74" spans="1:7">
       <c r="A74" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="B74" s="23" t="s">
@@ -2697,7 +2852,7 @@
     </row>
     <row r="75" spans="1:7">
       <c r="A75" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>61</v>
       </c>
       <c r="B75" s="23" t="s">
@@ -2713,7 +2868,7 @@
     </row>
     <row r="76" spans="1:7">
       <c r="A76" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>62</v>
       </c>
       <c r="B76" s="23" t="s">
@@ -2729,7 +2884,7 @@
     </row>
     <row r="77" spans="1:7">
       <c r="A77" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>63</v>
       </c>
       <c r="B77" s="23" t="s">
@@ -2745,7 +2900,7 @@
     </row>
     <row r="78" spans="1:7">
       <c r="A78" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="B78" s="23"/>
@@ -2757,7 +2912,7 @@
     </row>
     <row r="79" spans="1:7" s="42" customFormat="1">
       <c r="A79" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>65</v>
       </c>
       <c r="B79" s="23" t="s">
@@ -2773,7 +2928,7 @@
     </row>
     <row r="80" spans="1:7" s="42" customFormat="1">
       <c r="A80" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>66</v>
       </c>
       <c r="B80" s="23" t="s">
@@ -2789,14 +2944,14 @@
     </row>
     <row r="81" spans="1:7" s="42" customFormat="1">
       <c r="A81" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A81:A108" si="1">ROW() - 14</f>
         <v>67</v>
       </c>
       <c r="B81" s="23" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="C81" s="20" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D81" s="21"/>
       <c r="E81" s="21"/>
@@ -2809,189 +2964,199 @@
         <v>68</v>
       </c>
       <c r="B82" s="23" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="C82" s="20" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D82" s="21"/>
       <c r="E82" s="21"/>
       <c r="F82" s="21"/>
       <c r="G82" s="22"/>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" s="42" customFormat="1">
       <c r="A83" s="28">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="B83" s="23"/>
-      <c r="C83" s="20"/>
+      <c r="B83" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="C83" s="20" t="s">
+        <v>129</v>
+      </c>
       <c r="D83" s="21"/>
       <c r="E83" s="21"/>
       <c r="F83" s="21"/>
       <c r="G83" s="22"/>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" s="42" customFormat="1">
       <c r="A84" s="28">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="B84" s="23" t="s">
-        <v>71</v>
+        <v>136</v>
       </c>
       <c r="C84" s="20" t="s">
-        <v>87</v>
+        <v>130</v>
       </c>
       <c r="D84" s="21"/>
       <c r="E84" s="21"/>
       <c r="F84" s="21"/>
       <c r="G84" s="22"/>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" s="42" customFormat="1">
       <c r="A85" s="28">
         <f t="shared" si="1"/>
         <v>71</v>
       </c>
-      <c r="B85" s="23"/>
-      <c r="C85" s="20"/>
+      <c r="B85" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="C85" s="20" t="s">
+        <v>131</v>
+      </c>
       <c r="D85" s="21"/>
       <c r="E85" s="21"/>
       <c r="F85" s="21"/>
       <c r="G85" s="22"/>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" s="42" customFormat="1">
       <c r="A86" s="28">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-      <c r="B86" s="23"/>
+      <c r="B86" s="23" t="s">
+        <v>138</v>
+      </c>
       <c r="C86" s="20" t="s">
-        <v>72</v>
+        <v>132</v>
       </c>
       <c r="D86" s="21"/>
       <c r="E86" s="21"/>
       <c r="F86" s="21"/>
       <c r="G86" s="22"/>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" s="42" customFormat="1">
       <c r="A87" s="28">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
-      <c r="B87" s="23"/>
+      <c r="B87" s="23" t="s">
+        <v>139</v>
+      </c>
       <c r="C87" s="20" t="s">
-        <v>88</v>
+        <v>133</v>
       </c>
       <c r="D87" s="21"/>
       <c r="E87" s="21"/>
       <c r="F87" s="21"/>
       <c r="G87" s="22"/>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" s="42" customFormat="1">
       <c r="A88" s="28">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-      <c r="B88" s="23"/>
+      <c r="B88" s="23" t="s">
+        <v>141</v>
+      </c>
       <c r="C88" s="20" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
       <c r="D88" s="21"/>
       <c r="E88" s="21"/>
       <c r="F88" s="21"/>
       <c r="G88" s="22"/>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" s="42" customFormat="1">
       <c r="A89" s="28">
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
       <c r="B89" s="23" t="s">
-        <v>90</v>
+        <v>144</v>
       </c>
       <c r="C89" s="20" t="s">
-        <v>91</v>
+        <v>145</v>
       </c>
       <c r="D89" s="21"/>
       <c r="E89" s="21"/>
       <c r="F89" s="21"/>
       <c r="G89" s="22"/>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:7" s="42" customFormat="1">
       <c r="A90" s="28">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
       <c r="B90" s="23" t="s">
-        <v>92</v>
+        <v>142</v>
       </c>
       <c r="C90" s="20" t="s">
-        <v>93</v>
+        <v>146</v>
       </c>
       <c r="D90" s="21"/>
       <c r="E90" s="21"/>
       <c r="F90" s="21"/>
       <c r="G90" s="22"/>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" s="42" customFormat="1">
       <c r="A91" s="28">
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
       <c r="B91" s="23" t="s">
-        <v>94</v>
+        <v>143</v>
       </c>
       <c r="C91" s="20" t="s">
-        <v>95</v>
+        <v>147</v>
       </c>
       <c r="D91" s="21"/>
       <c r="E91" s="21"/>
       <c r="F91" s="21"/>
       <c r="G91" s="22"/>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" s="42" customFormat="1">
       <c r="A92" s="28">
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
       <c r="B92" s="23" t="s">
-        <v>96</v>
+        <v>148</v>
       </c>
       <c r="C92" s="20" t="s">
-        <v>97</v>
+        <v>149</v>
       </c>
       <c r="D92" s="21"/>
       <c r="E92" s="21"/>
       <c r="F92" s="21"/>
       <c r="G92" s="22"/>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" s="42" customFormat="1">
       <c r="A93" s="28">
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
       <c r="B93" s="23" t="s">
-        <v>98</v>
+        <v>150</v>
       </c>
       <c r="C93" s="20" t="s">
-        <v>99</v>
+        <v>151</v>
       </c>
       <c r="D93" s="21"/>
       <c r="E93" s="21"/>
       <c r="F93" s="21"/>
       <c r="G93" s="22"/>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" s="42" customFormat="1">
       <c r="A94" s="28">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="B94" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="C94" s="20" t="s">
-        <v>101</v>
-      </c>
+      <c r="B94" s="23"/>
+      <c r="C94" s="20"/>
       <c r="D94" s="21"/>
       <c r="E94" s="21"/>
       <c r="F94" s="21"/>
@@ -2999,15 +3164,11 @@
     </row>
     <row r="95" spans="1:7">
       <c r="A95" s="28">
-        <f t="shared" ref="A95:A96" si="2">ROW() - 14</f>
+        <f t="shared" si="1"/>
         <v>81</v>
       </c>
-      <c r="B95" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="C95" s="20" t="s">
-        <v>103</v>
-      </c>
+      <c r="B95" s="23"/>
+      <c r="C95" s="20"/>
       <c r="D95" s="21"/>
       <c r="E95" s="21"/>
       <c r="F95" s="21"/>
@@ -3015,14 +3176,14 @@
     </row>
     <row r="96" spans="1:7">
       <c r="A96" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>82</v>
       </c>
       <c r="B96" s="23" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="C96" s="20" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="D96" s="21"/>
       <c r="E96" s="21"/>
@@ -3030,22 +3191,204 @@
       <c r="G96" s="22"/>
     </row>
     <row r="97" spans="1:7">
-      <c r="A97" s="28"/>
+      <c r="A97" s="28">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
       <c r="B97" s="23"/>
       <c r="C97" s="20"/>
-      <c r="D97" s="34"/>
-      <c r="E97" s="34"/>
-      <c r="F97" s="34"/>
-      <c r="G97" s="35"/>
+      <c r="D97" s="21"/>
+      <c r="E97" s="21"/>
+      <c r="F97" s="21"/>
+      <c r="G97" s="22"/>
     </row>
     <row r="98" spans="1:7">
-      <c r="A98" s="29"/>
-      <c r="B98" s="24"/>
-      <c r="C98" s="25"/>
-      <c r="D98" s="26"/>
-      <c r="E98" s="26"/>
-      <c r="F98" s="26"/>
-      <c r="G98" s="27"/>
+      <c r="A98" s="28">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="B98" s="23"/>
+      <c r="C98" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D98" s="21"/>
+      <c r="E98" s="21"/>
+      <c r="F98" s="21"/>
+      <c r="G98" s="22"/>
+    </row>
+    <row r="99" spans="1:7">
+      <c r="A99" s="28">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="B99" s="23"/>
+      <c r="C99" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D99" s="21"/>
+      <c r="E99" s="21"/>
+      <c r="F99" s="21"/>
+      <c r="G99" s="22"/>
+    </row>
+    <row r="100" spans="1:7">
+      <c r="A100" s="28">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="B100" s="23"/>
+      <c r="C100" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D100" s="21"/>
+      <c r="E100" s="21"/>
+      <c r="F100" s="21"/>
+      <c r="G100" s="22"/>
+    </row>
+    <row r="101" spans="1:7">
+      <c r="A101" s="28">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="B101" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="C101" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D101" s="21"/>
+      <c r="E101" s="21"/>
+      <c r="F101" s="21"/>
+      <c r="G101" s="22"/>
+    </row>
+    <row r="102" spans="1:7">
+      <c r="A102" s="28">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="B102" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="C102" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D102" s="21"/>
+      <c r="E102" s="21"/>
+      <c r="F102" s="21"/>
+      <c r="G102" s="22"/>
+    </row>
+    <row r="103" spans="1:7">
+      <c r="A103" s="28">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="B103" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C103" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D103" s="21"/>
+      <c r="E103" s="21"/>
+      <c r="F103" s="21"/>
+      <c r="G103" s="22"/>
+    </row>
+    <row r="104" spans="1:7">
+      <c r="A104" s="28">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="B104" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C104" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D104" s="21"/>
+      <c r="E104" s="21"/>
+      <c r="F104" s="21"/>
+      <c r="G104" s="22"/>
+    </row>
+    <row r="105" spans="1:7">
+      <c r="A105" s="28">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="B105" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="C105" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="D105" s="21"/>
+      <c r="E105" s="21"/>
+      <c r="F105" s="21"/>
+      <c r="G105" s="22"/>
+    </row>
+    <row r="106" spans="1:7">
+      <c r="A106" s="28">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="B106" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="C106" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D106" s="21"/>
+      <c r="E106" s="21"/>
+      <c r="F106" s="21"/>
+      <c r="G106" s="22"/>
+    </row>
+    <row r="107" spans="1:7">
+      <c r="A107" s="28">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+      <c r="B107" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="C107" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="D107" s="21"/>
+      <c r="E107" s="21"/>
+      <c r="F107" s="21"/>
+      <c r="G107" s="22"/>
+    </row>
+    <row r="108" spans="1:7">
+      <c r="A108" s="28">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="B108" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C108" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D108" s="21"/>
+      <c r="E108" s="21"/>
+      <c r="F108" s="21"/>
+      <c r="G108" s="22"/>
+    </row>
+    <row r="109" spans="1:7">
+      <c r="A109" s="28"/>
+      <c r="B109" s="23"/>
+      <c r="C109" s="20"/>
+      <c r="D109" s="34"/>
+      <c r="E109" s="34"/>
+      <c r="F109" s="34"/>
+      <c r="G109" s="35"/>
+    </row>
+    <row r="110" spans="1:7">
+      <c r="A110" s="29"/>
+      <c r="B110" s="24"/>
+      <c r="C110" s="25"/>
+      <c r="D110" s="26"/>
+      <c r="E110" s="26"/>
+      <c r="F110" s="26"/>
+      <c r="G110" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
1.0.1: keep i18n instance in ValidateConfig class statically.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoVeeValidateResourceBundle.xlsx
+++ b/meta/program/BlancoVeeValidateResourceBundle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoVeeValidate/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DB32C4-27BF-9745-9655-08F7A7A81489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61E0E06-3B5A-0F46-811C-FDE779DB45FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23360" yWindow="8800" windowWidth="28800" windowHeight="17540" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22400" yWindow="8800" windowWidth="28800" windowHeight="17540" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ja" sheetId="9" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="154">
   <si>
     <t>説明</t>
     <rPh sb="0" eb="2">
@@ -877,6 +877,17 @@
     </rPh>
     <rPh sb="21" eb="23">
       <t xml:space="preserve">テイギ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XML2SOURCE_FILE.VALIDATE.INIT.I18N</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>vue-i18nのインスタンスを保持します。</t>
+    <rPh sb="16" eb="18">
+      <t xml:space="preserve">ホジシマス。 </t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1813,10 +1824,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I110"/>
+  <dimension ref="A1:I111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1985,7 +1996,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="28">
-        <f t="shared" ref="A17:A80" si="0">ROW() - 14</f>
+        <f t="shared" ref="A17:A81" si="0">ROW() - 14</f>
         <v>3</v>
       </c>
       <c r="B17" s="23"/>
@@ -2944,14 +2955,14 @@
     </row>
     <row r="81" spans="1:7" s="42" customFormat="1">
       <c r="A81" s="28">
-        <f t="shared" ref="A81:A108" si="1">ROW() - 14</f>
+        <f t="shared" si="0"/>
         <v>67</v>
       </c>
       <c r="B81" s="23" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
       <c r="C81" s="20" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="D81" s="21"/>
       <c r="E81" s="21"/>
@@ -2960,14 +2971,14 @@
     </row>
     <row r="82" spans="1:7" s="42" customFormat="1">
       <c r="A82" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A82:A109" si="1">ROW() - 14</f>
         <v>68</v>
       </c>
       <c r="B82" s="23" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C82" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D82" s="21"/>
       <c r="E82" s="21"/>
@@ -2980,10 +2991,10 @@
         <v>69</v>
       </c>
       <c r="B83" s="23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C83" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D83" s="21"/>
       <c r="E83" s="21"/>
@@ -2996,10 +3007,10 @@
         <v>70</v>
       </c>
       <c r="B84" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C84" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D84" s="21"/>
       <c r="E84" s="21"/>
@@ -3012,10 +3023,10 @@
         <v>71</v>
       </c>
       <c r="B85" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C85" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D85" s="21"/>
       <c r="E85" s="21"/>
@@ -3028,10 +3039,10 @@
         <v>72</v>
       </c>
       <c r="B86" s="23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C86" s="20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D86" s="21"/>
       <c r="E86" s="21"/>
@@ -3044,10 +3055,10 @@
         <v>73</v>
       </c>
       <c r="B87" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C87" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D87" s="21"/>
       <c r="E87" s="21"/>
@@ -3060,10 +3071,10 @@
         <v>74</v>
       </c>
       <c r="B88" s="23" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C88" s="20" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="D88" s="21"/>
       <c r="E88" s="21"/>
@@ -3076,10 +3087,10 @@
         <v>75</v>
       </c>
       <c r="B89" s="23" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C89" s="20" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D89" s="21"/>
       <c r="E89" s="21"/>
@@ -3092,10 +3103,10 @@
         <v>76</v>
       </c>
       <c r="B90" s="23" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C90" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D90" s="21"/>
       <c r="E90" s="21"/>
@@ -3108,10 +3119,10 @@
         <v>77</v>
       </c>
       <c r="B91" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C91" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D91" s="21"/>
       <c r="E91" s="21"/>
@@ -3124,10 +3135,10 @@
         <v>78</v>
       </c>
       <c r="B92" s="23" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C92" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D92" s="21"/>
       <c r="E92" s="21"/>
@@ -3140,10 +3151,10 @@
         <v>79</v>
       </c>
       <c r="B93" s="23" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C93" s="20" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D93" s="21"/>
       <c r="E93" s="21"/>
@@ -3155,14 +3166,18 @@
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="B94" s="23"/>
-      <c r="C94" s="20"/>
+      <c r="B94" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="C94" s="20" t="s">
+        <v>151</v>
+      </c>
       <c r="D94" s="21"/>
       <c r="E94" s="21"/>
       <c r="F94" s="21"/>
       <c r="G94" s="22"/>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" s="42" customFormat="1">
       <c r="A95" s="28">
         <f t="shared" si="1"/>
         <v>81</v>
@@ -3179,12 +3194,8 @@
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
-      <c r="B96" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="C96" s="20" t="s">
-        <v>87</v>
-      </c>
+      <c r="B96" s="23"/>
+      <c r="C96" s="20"/>
       <c r="D96" s="21"/>
       <c r="E96" s="21"/>
       <c r="F96" s="21"/>
@@ -3195,8 +3206,12 @@
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
-      <c r="B97" s="23"/>
-      <c r="C97" s="20"/>
+      <c r="B97" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C97" s="20" t="s">
+        <v>87</v>
+      </c>
       <c r="D97" s="21"/>
       <c r="E97" s="21"/>
       <c r="F97" s="21"/>
@@ -3208,9 +3223,7 @@
         <v>84</v>
       </c>
       <c r="B98" s="23"/>
-      <c r="C98" s="20" t="s">
-        <v>72</v>
-      </c>
+      <c r="C98" s="20"/>
       <c r="D98" s="21"/>
       <c r="E98" s="21"/>
       <c r="F98" s="21"/>
@@ -3223,7 +3236,7 @@
       </c>
       <c r="B99" s="23"/>
       <c r="C99" s="20" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="D99" s="21"/>
       <c r="E99" s="21"/>
@@ -3237,7 +3250,7 @@
       </c>
       <c r="B100" s="23"/>
       <c r="C100" s="20" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="D100" s="21"/>
       <c r="E100" s="21"/>
@@ -3249,11 +3262,9 @@
         <f t="shared" si="1"/>
         <v>87</v>
       </c>
-      <c r="B101" s="23" t="s">
-        <v>90</v>
-      </c>
+      <c r="B101" s="23"/>
       <c r="C101" s="20" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="D101" s="21"/>
       <c r="E101" s="21"/>
@@ -3266,10 +3277,10 @@
         <v>88</v>
       </c>
       <c r="B102" s="23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C102" s="20" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D102" s="21"/>
       <c r="E102" s="21"/>
@@ -3282,10 +3293,10 @@
         <v>89</v>
       </c>
       <c r="B103" s="23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C103" s="20" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D103" s="21"/>
       <c r="E103" s="21"/>
@@ -3298,10 +3309,10 @@
         <v>90</v>
       </c>
       <c r="B104" s="23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C104" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D104" s="21"/>
       <c r="E104" s="21"/>
@@ -3314,10 +3325,10 @@
         <v>91</v>
       </c>
       <c r="B105" s="23" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C105" s="20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D105" s="21"/>
       <c r="E105" s="21"/>
@@ -3330,10 +3341,10 @@
         <v>92</v>
       </c>
       <c r="B106" s="23" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C106" s="20" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D106" s="21"/>
       <c r="E106" s="21"/>
@@ -3346,10 +3357,10 @@
         <v>93</v>
       </c>
       <c r="B107" s="23" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C107" s="20" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D107" s="21"/>
       <c r="E107" s="21"/>
@@ -3362,10 +3373,10 @@
         <v>94</v>
       </c>
       <c r="B108" s="23" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="C108" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D108" s="21"/>
       <c r="E108" s="21"/>
@@ -3373,22 +3384,38 @@
       <c r="G108" s="22"/>
     </row>
     <row r="109" spans="1:7">
-      <c r="A109" s="28"/>
-      <c r="B109" s="23"/>
-      <c r="C109" s="20"/>
-      <c r="D109" s="34"/>
-      <c r="E109" s="34"/>
-      <c r="F109" s="34"/>
-      <c r="G109" s="35"/>
+      <c r="A109" s="28">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="B109" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C109" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D109" s="21"/>
+      <c r="E109" s="21"/>
+      <c r="F109" s="21"/>
+      <c r="G109" s="22"/>
     </row>
     <row r="110" spans="1:7">
-      <c r="A110" s="29"/>
-      <c r="B110" s="24"/>
-      <c r="C110" s="25"/>
-      <c r="D110" s="26"/>
-      <c r="E110" s="26"/>
-      <c r="F110" s="26"/>
-      <c r="G110" s="27"/>
+      <c r="A110" s="28"/>
+      <c r="B110" s="23"/>
+      <c r="C110" s="20"/>
+      <c r="D110" s="34"/>
+      <c r="E110" s="34"/>
+      <c r="F110" s="34"/>
+      <c r="G110" s="35"/>
+    </row>
+    <row r="111" spans="1:7">
+      <c r="A111" s="29"/>
+      <c r="B111" s="24"/>
+      <c r="C111" s="25"/>
+      <c r="D111" s="26"/>
+      <c r="E111" s="26"/>
+      <c r="F111" s="26"/>
+      <c r="G111" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>